<commit_message>
Add release/1.0.0 to meta-sheet
</commit_message>
<xml_diff>
--- a/meta-sheet.xlsx
+++ b/meta-sheet.xlsx
@@ -1,63 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MS LAKSHMI\Documents\DevSecOps\src\zdt-manager-src\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D6F7998-F371-415F-B7E1-E6441004F536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{2FF642BF-C88A-4981-B434-E25CE7310D65}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
-  <si>
-    <t>dev</t>
-  </si>
-  <si>
-    <t>sit</t>
-  </si>
-  <si>
-    <t>uat</t>
-  </si>
-  <si>
-    <t>prod</t>
-  </si>
-  <si>
-    <t>main</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -76,21 +46,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -390,41 +419,83 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BB5C185-C768-4AA4-8C90-4451765C3B89}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>dev</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>sit</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>uat</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>prod</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>main</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>main</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>main</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>main</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>release/1.0.0</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add release/1.0.1 to meta-sheet
</commit_message>
<xml_diff>
--- a/meta-sheet.xlsx
+++ b/meta-sheet.xlsx
@@ -1,53 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
-  <si>
-    <t>dev</t>
-  </si>
-  <si>
-    <t>sit</t>
-  </si>
-  <si>
-    <t>uat</t>
-  </si>
-  <si>
-    <t>prod</t>
-  </si>
-  <si>
-    <t>release/1.0.0</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -66,24 +46,86 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -371,48 +413,89 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="1" max="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="3" max="3"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
+    <row r="1" ht="18.75" customHeight="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>dev</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>sit</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>uat</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>prod</t>
+        </is>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>4</v>
+    <row r="2" ht="18.75" customHeight="1">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>release/1.0.0</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>release/1.0.0</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>release/1.0.0</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>release/1.0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>release/1.0.1</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add release/1.0.2 to meta-sheet
</commit_message>
<xml_diff>
--- a/meta-sheet.xlsx
+++ b/meta-sheet.xlsx
@@ -1,58 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\himan\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC2E9FD4-173E-4741-AC9C-FBA97A4DB012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="2160" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2160" yWindow="2160" windowWidth="17280" windowHeight="8880" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
-  <si>
-    <t>prod</t>
-  </si>
-  <si>
-    <t>dev</t>
-  </si>
-  <si>
-    <t>sit</t>
-  </si>
-  <si>
-    <t>uat</t>
-  </si>
-  <si>
-    <t>release/1.0.0</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -71,21 +46,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -373,50 +407,89 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col width="15" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="16.33203125" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="19.88671875" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="17.44140625" bestFit="1" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>0</v>
+    <row r="1" ht="18.75" customHeight="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>dev</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>sit</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>uat</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>prod</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
+    <row r="2" ht="18.75" customHeight="1">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>release/1.0.0</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>release/1.0.0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>release/1.0.0</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>release/1.0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>release/1.0.2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Promote release/1.0.2 from uat to mig
</commit_message>
<xml_diff>
--- a/meta-sheet.xlsx
+++ b/meta-sheet.xlsx
@@ -1,76 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\himan\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4201521-2D09-4EB6-9483-9A8D42D556EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="11">
-  <si>
-    <t>prod</t>
-  </si>
-  <si>
-    <t>dev</t>
-  </si>
-  <si>
-    <t>sit</t>
-  </si>
-  <si>
-    <t>uat</t>
-  </si>
-  <si>
-    <t>main</t>
-  </si>
-  <si>
-    <t>mig</t>
-  </si>
-  <si>
-    <t>pre-prod</t>
-  </si>
-  <si>
-    <t>release/1.0.0</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>release/1.0.1</t>
-  </si>
-  <si>
-    <t>release/1.0.2</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -89,21 +46,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -391,9 +407,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
+    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:F5"/>
   <sheetViews>
@@ -401,112 +418,172 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col width="15" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="16.33203125" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="19.88671875" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="17.44140625" bestFit="1" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>0</v>
+    <row r="1" ht="18.75" customHeight="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>dev</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>sit</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>uat</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>mig</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>pre-prod</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>prod</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>4</v>
+    <row r="2" ht="18.75" customHeight="1">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>main</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>main</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>main</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>main</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>main</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>main</t>
+        </is>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" t="s">
-        <v>8</v>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>release/1.0.0</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>release/1.0.0</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" t="s">
-        <v>8</v>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>release/1.0.1</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>release/1.0.1</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" t="s">
-        <v>8</v>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>release/1.0.2</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>release/1.0.2</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>release/1.0.2</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>release/1.0.2</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add release/1.0.3 to meta-sheet
</commit_message>
<xml_diff>
--- a/meta-sheet.xlsx
+++ b/meta-sheet.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
@@ -586,6 +586,38 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>release/1.0.3</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add release/1.1.0 to meta-sheet
</commit_message>
<xml_diff>
--- a/meta-sheet.xlsx
+++ b/meta-sheet.xlsx
@@ -1,70 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\himan\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFE7F36E-6056-4493-98B8-307BE2E953B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
-  <si>
-    <t>prod</t>
-  </si>
-  <si>
-    <t>dev</t>
-  </si>
-  <si>
-    <t>sit</t>
-  </si>
-  <si>
-    <t>uat</t>
-  </si>
-  <si>
-    <t>main</t>
-  </si>
-  <si>
-    <t>mig</t>
-  </si>
-  <si>
-    <t>pre-prod</t>
-  </si>
-  <si>
-    <t>release/1.0.0</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -83,21 +46,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -385,82 +407,151 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col width="15" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="16.33203125" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="19.88671875" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="17.44140625" bestFit="1" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>0</v>
+    <row r="1" ht="18.75" customHeight="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>dev</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>sit</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>uat</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>mig</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>pre-prod</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>prod</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>4</v>
+    <row r="2" ht="18.75" customHeight="1">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>main</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>main</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>main</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>main</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>main</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>main</t>
+        </is>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" t="s">
-        <v>8</v>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>release/1.0.0</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>release/1.0.0</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>release/1.1.0</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add release/1.1.1 to meta-sheet
</commit_message>
<xml_diff>
--- a/meta-sheet.xlsx
+++ b/meta-sheet.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
@@ -554,6 +554,38 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>release/1.1.1</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add release/release/1.0.3 to meta-sheet
</commit_message>
<xml_diff>
--- a/meta-sheet.xlsx
+++ b/meta-sheet.xlsx
@@ -1,73 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\himan\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7DDEF6E-A8A7-482D-A68F-16D071BF322E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="8880" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="10">
-  <si>
-    <t>prod</t>
-  </si>
-  <si>
-    <t>dev</t>
-  </si>
-  <si>
-    <t>sit</t>
-  </si>
-  <si>
-    <t>uat</t>
-  </si>
-  <si>
-    <t>main</t>
-  </si>
-  <si>
-    <t>mig</t>
-  </si>
-  <si>
-    <t>pre-prod</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>release/1.0.1</t>
-  </si>
-  <si>
-    <t>release/1.0.2</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -86,21 +46,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -388,102 +407,183 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col width="15" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="16.33203125" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="19.88671875" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="17.44140625" bestFit="1" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>0</v>
+    <row r="1" ht="18.75" customHeight="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>dev</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>sit</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>uat</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>mig</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>pre-prod</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>prod</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>4</v>
+    <row r="2" ht="18.75" customHeight="1">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>main</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>main</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>main</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>main</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>main</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>main</t>
+        </is>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" t="s">
-        <v>7</v>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>release/1.0.1</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>release/1.0.1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" t="s">
-        <v>7</v>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>release/1.0.2</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>release/1.0.2</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>release/release/1.0.3</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add release/1.0.4 to meta-sheet
</commit_message>
<xml_diff>
--- a/meta-sheet.xlsx
+++ b/meta-sheet.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
@@ -586,6 +586,38 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>release/1.0.4</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add release/1.0.5 to meta-sheet
</commit_message>
<xml_diff>
--- a/meta-sheet.xlsx
+++ b/meta-sheet.xlsx
@@ -1,79 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\himan\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C85E4B1-8DDE-4E64-BE6F-D0868E5C41A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="12">
-  <si>
-    <t>prod</t>
-  </si>
-  <si>
-    <t>dev</t>
-  </si>
-  <si>
-    <t>sit</t>
-  </si>
-  <si>
-    <t>uat</t>
-  </si>
-  <si>
-    <t>main</t>
-  </si>
-  <si>
-    <t>mig</t>
-  </si>
-  <si>
-    <t>pre-prod</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>release/1.0.1</t>
-  </si>
-  <si>
-    <t>release/1.0.2</t>
-  </si>
-  <si>
-    <t>release/1.0.3</t>
-  </si>
-  <si>
-    <t>release/1.0.4</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -92,22 +46,81 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -395,142 +408,247 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col width="15" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
+    <col width="16.33203125" bestFit="1" customWidth="1" style="1" min="2" max="2"/>
+    <col width="19.88671875" bestFit="1" customWidth="1" style="1" min="3" max="3"/>
+    <col width="17.44140625" bestFit="1" customWidth="1" style="1" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>0</v>
+    <row r="1" ht="18.75" customHeight="1" s="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>dev</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>sit</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>uat</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>mig</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>pre-prod</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>prod</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>4</v>
+    <row r="2" ht="18.75" customHeight="1" s="1">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>main</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>main</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>main</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>main</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>main</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>main</t>
+        </is>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" t="s">
-        <v>7</v>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>release/1.0.1</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>release/1.0.1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" t="s">
-        <v>7</v>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>release/1.0.2</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>release/1.0.2</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>7</v>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>release/1.0.3</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>release/1.0.3</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>7</v>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>release/1.0.4</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>release/1.0.4</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>release/1.0.5</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add release/6.0.0 to meta-sheet
</commit_message>
<xml_diff>
--- a/meta-sheet.xlsx
+++ b/meta-sheet.xlsx
@@ -1,58 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MS LAKSHMI\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEBBA813-B172-4C40-90C8-553C1574CAA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
-  <si>
-    <t>prod</t>
-  </si>
-  <si>
-    <t>dev</t>
-  </si>
-  <si>
-    <t>sit</t>
-  </si>
-  <si>
-    <t>uat</t>
-  </si>
-  <si>
-    <t>main</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -71,21 +46,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -373,50 +407,89 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.453125" bestFit="1" customWidth="1"/>
+    <col width="15" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="16.36328125" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="19.90625" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="17.453125" bestFit="1" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>0</v>
+    <row r="1" ht="18.75" customHeight="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>dev</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>sit</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>uat</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>prod</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
+    <row r="2" ht="18.75" customHeight="1">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>main</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>main</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>main</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>main</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>release/6.0.0</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add release/8.0.0 to meta-sheet
</commit_message>
<xml_diff>
--- a/meta-sheet.xlsx
+++ b/meta-sheet.xlsx
@@ -1,58 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MS LAKSHMI\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEBBA813-B172-4C40-90C8-553C1574CAA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
-  <si>
-    <t>prod</t>
-  </si>
-  <si>
-    <t>dev</t>
-  </si>
-  <si>
-    <t>sit</t>
-  </si>
-  <si>
-    <t>uat</t>
-  </si>
-  <si>
-    <t>main</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -71,21 +46,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -373,50 +407,89 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.453125" bestFit="1" customWidth="1"/>
+    <col width="15" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="16.36328125" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="19.90625" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="17.453125" bestFit="1" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>0</v>
+    <row r="1" ht="18.75" customHeight="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>dev</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>sit</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>uat</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>prod</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
+    <row r="2" ht="18.75" customHeight="1">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>main</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>main</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>main</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>main</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>release/8.0.0</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add release/8.0.2 to meta-sheet
</commit_message>
<xml_diff>
--- a/meta-sheet.xlsx
+++ b/meta-sheet.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -492,6 +492,28 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>release/8.0.2</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add release/8.0.3 to meta-sheet
</commit_message>
<xml_diff>
--- a/meta-sheet.xlsx
+++ b/meta-sheet.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -514,6 +514,28 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>release/8.0.3</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add release/8.0.1 to meta-sheet
</commit_message>
<xml_diff>
--- a/meta-sheet.xlsx
+++ b/meta-sheet.xlsx
@@ -1,64 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\himan\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC671046-AC9E-4286-9CBF-3675618CAED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
-  <si>
-    <t>prod</t>
-  </si>
-  <si>
-    <t>dev</t>
-  </si>
-  <si>
-    <t>sit</t>
-  </si>
-  <si>
-    <t>uat</t>
-  </si>
-  <si>
-    <t>main</t>
-  </si>
-  <si>
-    <t>pre-prod</t>
-  </si>
-  <si>
-    <t>release/8.0.0</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -77,22 +46,81 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -380,74 +408,132 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" customWidth="1"/>
+    <col width="15" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
+    <col width="16.33203125" bestFit="1" customWidth="1" style="1" min="2" max="2"/>
+    <col width="19.88671875" bestFit="1" customWidth="1" style="1" min="3" max="3"/>
+    <col width="12.33203125" customWidth="1" style="1" min="4" max="4"/>
+    <col width="17.33203125" customWidth="1" style="1" min="5" max="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>0</v>
+    <row r="1" ht="18.75" customHeight="1" s="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>dev</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>sit</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>uat</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>pre-prod</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>prod</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
+    <row r="2" ht="18.75" customHeight="1" s="1">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>main</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>main</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>main</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>main</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>main</t>
+        </is>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>6</v>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>release/8.0.0</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>release/8.0.0</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>release/8.0.0</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>release/8.0.0</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>release/8.0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>release/8.0.1</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Promoted release/8.0.0 from sit to uat
</commit_message>
<xml_diff>
--- a/meta-sheet.xlsx
+++ b/meta-sheet.xlsx
@@ -1,67 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\himan\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67FA62E9-9219-4C0E-97A4-22011C807D57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
-  <si>
-    <t>prod</t>
-  </si>
-  <si>
-    <t>dev</t>
-  </si>
-  <si>
-    <t>sit</t>
-  </si>
-  <si>
-    <t>uat</t>
-  </si>
-  <si>
-    <t>main</t>
-  </si>
-  <si>
-    <t>pre-prod</t>
-  </si>
-  <si>
-    <t>release/8.0.0</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -80,21 +46,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -382,9 +407,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
+    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -392,64 +418,94 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" customWidth="1"/>
+    <col width="15" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="16.33203125" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="19.88671875" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="12.33203125" customWidth="1" min="4" max="4"/>
+    <col width="17.33203125" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>0</v>
+    <row r="1" ht="18.75" customHeight="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>dev</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>sit</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>uat</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>pre-prod</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>prod</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
+    <row r="2" ht="18.75" customHeight="1">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>main</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>main</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>main</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>main</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>main</t>
+        </is>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>release/8.0.0</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>release/8.0.0</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>release/8.0.0</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add release/8.0.4 to meta-sheet
</commit_message>
<xml_diff>
--- a/meta-sheet.xlsx
+++ b/meta-sheet.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
@@ -589,6 +589,33 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>release/8.0.4</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add release/8.0.5 to meta-sheet
</commit_message>
<xml_diff>
--- a/meta-sheet.xlsx
+++ b/meta-sheet.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
@@ -616,6 +616,33 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>release/8.0.5</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add release/8.0.6 to meta-sheet
</commit_message>
<xml_diff>
--- a/meta-sheet.xlsx
+++ b/meta-sheet.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
@@ -643,6 +643,33 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>release/8.0.6</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add release/8.0.7 to meta-sheet
</commit_message>
<xml_diff>
--- a/meta-sheet.xlsx
+++ b/meta-sheet.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
@@ -670,6 +670,33 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>release/8.0.7</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add release/8.0.8 to meta-sheet
</commit_message>
<xml_diff>
--- a/meta-sheet.xlsx
+++ b/meta-sheet.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
@@ -697,6 +697,33 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>release/8.0.8</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add release/8.0.9 to meta-sheet
</commit_message>
<xml_diff>
--- a/meta-sheet.xlsx
+++ b/meta-sheet.xlsx
@@ -418,7 +418,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -730,6 +730,33 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>release/8.0.9</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add release/8.0.10 to meta-sheet
</commit_message>
<xml_diff>
--- a/meta-sheet.xlsx
+++ b/meta-sheet.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K12" sqref="K12"/>
@@ -751,6 +751,33 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>release/8.0.10</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add release/8.0.11 to meta-sheet
</commit_message>
<xml_diff>
--- a/meta-sheet.xlsx
+++ b/meta-sheet.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A13" sqref="A13:XFD13"/>
@@ -778,6 +778,33 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>release/8.0.11</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add release/release/8.0.12 to meta-sheet
</commit_message>
<xml_diff>
--- a/meta-sheet.xlsx
+++ b/meta-sheet.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
@@ -805,6 +805,33 @@
         </is>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>release/release/8.0.12</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add release/8.0.14 to meta-sheet
</commit_message>
<xml_diff>
--- a/meta-sheet.xlsx
+++ b/meta-sheet.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
@@ -859,6 +859,33 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>release/8.0.14</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add release/8.0.15 to meta-sheet
</commit_message>
<xml_diff>
--- a/meta-sheet.xlsx
+++ b/meta-sheet.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
@@ -886,6 +886,33 @@
         </is>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>release/8.0.15</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add release/8.0.16 to meta-sheet
</commit_message>
<xml_diff>
--- a/meta-sheet.xlsx
+++ b/meta-sheet.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
@@ -913,6 +913,33 @@
         </is>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>release/8.0.16</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add release/8.0.17 to meta-sheet
</commit_message>
<xml_diff>
--- a/meta-sheet.xlsx
+++ b/meta-sheet.xlsx
@@ -418,7 +418,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -946,6 +946,33 @@
         </is>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>release/8.0.17</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>